<commit_message>
update filtering and template
</commit_message>
<xml_diff>
--- a/Projects/INBEVTRADMX/Data/inbevtradmx_template_6.xlsx
+++ b/Projects/INBEVTRADMX/Data/inbevtradmx_template_6.xlsx
@@ -19,6 +19,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">template!$A$1:$V$64</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">template!$A$1:$V$64</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">template!$A$1:$V$64</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">template!$A$1:$V$64</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -299,7 +300,7 @@
     <t xml:space="preserve">Promociones Vigente</t>
   </si>
   <si>
-    <t xml:space="preserve">Set FRIA Modreloramas</t>
+    <t xml:space="preserve">Set FRIA Moderloramas</t>
   </si>
   <si>
     <t xml:space="preserve">MODELORAMA</t>
@@ -835,22 +836,22 @@
   </sheetPr>
   <dimension ref="A1:V64"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="54.1326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.9081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="15" min="4" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="31.4540816326531"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="53.4591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.3673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="15" min="4" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="1" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3152,7 +3153,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>89</v>
       </c>
@@ -3208,7 +3209,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>89</v>
       </c>
@@ -3265,7 +3266,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>89</v>
       </c>
@@ -3330,7 +3331,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>89</v>
       </c>
@@ -3395,7 +3396,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>89</v>
       </c>
@@ -3452,7 +3453,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>89</v>
       </c>
@@ -3509,7 +3510,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>89</v>
       </c>
@@ -3566,7 +3567,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>89</v>
       </c>
@@ -3623,7 +3624,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>89</v>
       </c>
@@ -3688,7 +3689,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>89</v>
       </c>
@@ -3753,7 +3754,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>89</v>
       </c>
@@ -3813,7 +3814,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>89</v>
       </c>
@@ -3873,7 +3874,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>89</v>
       </c>
@@ -3933,7 +3934,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>89</v>
       </c>
@@ -3993,7 +3994,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>89</v>
       </c>
@@ -4053,7 +4054,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>89</v>
       </c>
@@ -4113,7 +4114,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>89</v>
       </c>
@@ -4173,7 +4174,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>89</v>
       </c>
@@ -4229,7 +4230,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>89</v>
       </c>
@@ -4289,7 +4290,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>89</v>
       </c>
@@ -4405,7 +4406,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>89</v>
       </c>
@@ -4459,7 +4460,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>89</v>
       </c>
@@ -4513,7 +4514,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>89</v>
       </c>
@@ -4575,7 +4576,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>89</v>
       </c>
@@ -4637,7 +4638,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>89</v>
       </c>
@@ -4786,6 +4787,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
@@ -4910,6 +4914,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>